<commit_message>
added print cut versions
</commit_message>
<xml_diff>
--- a/spreadsheet/world_cup_2018.xlsx
+++ b/spreadsheet/world_cup_2018.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denys\Dropbox\toodoom\worldcup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="1" activeTab="2" xr2:uid="{06679F38-40B3-4A34-860F-690D3A58D83C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28340" windowHeight="15300" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="T" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Settings" sheetId="2" r:id="rId2"/>
     <sheet name="2018 World Cup" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="db_fifarank">Settings!$B$17:$C$48</definedName>
@@ -25,8 +21,11 @@
     <definedName name="T">T!$1:$1048576</definedName>
     <definedName name="teams">Settings!$I$17:$I$48</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4451" uniqueCount="2560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4491" uniqueCount="2561">
   <si>
     <t>English</t>
   </si>
@@ -7717,17 +7716,20 @@
   </si>
   <si>
     <t>سعودی عرب</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode=";;;"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7860,6 +7862,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -8654,14 +8668,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8669,29 +8683,29 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -8701,7 +8715,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -8709,23 +8723,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -8733,14 +8747,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8748,19 +8762,19 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8769,28 +8783,28 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -8798,10 +8812,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -8811,30 +8825,32 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="59" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -9246,90 +9262,6 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -9410,8 +9342,98 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -10296,7 +10318,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{782D1F7B-CF0A-41E6-9288-EB4175BF7539}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{782D1F7B-CF0A-41E6-9288-EB4175BF7539}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10346,7 +10368,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A074EA50-1E57-40E6-851F-CA0EBD5346A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A074EA50-1E57-40E6-851F-CA0EBD5346A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10396,7 +10418,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F020D312-7BC3-4FBD-AB9E-A9719935489C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F020D312-7BC3-4FBD-AB9E-A9719935489C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10446,7 +10468,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FF0393A-621D-42D6-9296-5F6C72936D05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8FF0393A-621D-42D6-9296-5F6C72936D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10496,7 +10518,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93FF5326-1E09-47F7-8728-D0C1EDCDD414}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93FF5326-1E09-47F7-8728-D0C1EDCDD414}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10546,7 +10568,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D26A5583-6F72-424C-9841-654CCA231C94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D26A5583-6F72-424C-9841-654CCA231C94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10596,7 +10618,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544404A8-C949-4303-B512-2DD6D2E58DF6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{544404A8-C949-4303-B512-2DD6D2E58DF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10646,7 +10668,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD67162D-EC15-4017-A67B-0BFB58ADA516}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD67162D-EC15-4017-A67B-0BFB58ADA516}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10696,7 +10718,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E350EA3-E56D-44C1-821A-98392C4744FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E350EA3-E56D-44C1-821A-98392C4744FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10746,7 +10768,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9DDC49-9DD8-43CB-9687-395B464F3433}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5C9DDC49-9DD8-43CB-9687-395B464F3433}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10796,7 +10818,7 @@
         <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94574D24-6927-4705-B0D1-CF432FF5A178}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{94574D24-6927-4705-B0D1-CF432FF5A178}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10846,7 +10868,7 @@
         <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{907F9C8A-37F1-41EA-830E-5B6DA553A628}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{907F9C8A-37F1-41EA-830E-5B6DA553A628}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10896,7 +10918,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B758F92B-13BF-4E34-BBDF-057A37F5A6D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B758F92B-13BF-4E34-BBDF-057A37F5A6D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10946,7 +10968,7 @@
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C7C7E3F-C397-46B4-80E5-E01A13897BE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C7C7E3F-C397-46B4-80E5-E01A13897BE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10996,7 +11018,7 @@
         <xdr:cNvPr id="23" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8A180D-4650-4A37-BFAB-CE482E9729D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E8A180D-4650-4A37-BFAB-CE482E9729D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11046,7 +11068,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CEF2871-1DC4-467D-88D6-19312A379FCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7CEF2871-1DC4-467D-88D6-19312A379FCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11096,7 +11118,7 @@
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E4D3EF1-7C37-484B-BF7F-7419829506E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E4D3EF1-7C37-484B-BF7F-7419829506E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11146,7 +11168,7 @@
         <xdr:cNvPr id="27" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F427A27E-B507-49F5-B9FD-8022163B2682}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F427A27E-B507-49F5-B9FD-8022163B2682}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11196,7 +11218,7 @@
         <xdr:cNvPr id="25" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{469088DB-5DF4-4A2B-B7C2-9A55EED56FFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{469088DB-5DF4-4A2B-B7C2-9A55EED56FFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11246,7 +11268,7 @@
         <xdr:cNvPr id="30" name="Picture 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{430DB9D2-C059-44FC-912C-20B8AF11987A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{430DB9D2-C059-44FC-912C-20B8AF11987A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11296,7 +11318,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20BA7981-FAB6-48F3-9D3C-1FFF5BAE22F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20BA7981-FAB6-48F3-9D3C-1FFF5BAE22F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11346,7 +11368,7 @@
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8911F8B-EFB5-4EAF-9BCF-52B74B176C62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8911F8B-EFB5-4EAF-9BCF-52B74B176C62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11396,7 +11418,7 @@
         <xdr:cNvPr id="34" name="Picture 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9AE9F33-B65B-479A-B4AC-45E521F3192B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B9AE9F33-B65B-479A-B4AC-45E521F3192B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11446,7 +11468,7 @@
         <xdr:cNvPr id="35" name="Picture 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E03EFE6-6F0A-42E4-9B18-4EE68916BFBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E03EFE6-6F0A-42E4-9B18-4EE68916BFBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11496,7 +11518,7 @@
         <xdr:cNvPr id="33" name="Picture 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34E832B8-E97E-4A62-95AC-8B1007A62204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{34E832B8-E97E-4A62-95AC-8B1007A62204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11546,7 +11568,7 @@
         <xdr:cNvPr id="38" name="Picture 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD3E60C5-3004-45D9-86DC-AEAECCDB9D78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD3E60C5-3004-45D9-86DC-AEAECCDB9D78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11596,7 +11618,7 @@
         <xdr:cNvPr id="39" name="Picture 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96520393-3B3A-4783-989C-AC1B55C8EE1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96520393-3B3A-4783-989C-AC1B55C8EE1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11646,7 +11668,7 @@
         <xdr:cNvPr id="37" name="Picture 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86F25E43-2711-437F-BA14-DE451A8343E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{86F25E43-2711-437F-BA14-DE451A8343E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11696,7 +11718,7 @@
         <xdr:cNvPr id="42" name="Picture 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E8E43E5-63FB-435A-AF15-FFDA7DBD257A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0E8E43E5-63FB-435A-AF15-FFDA7DBD257A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11746,7 +11768,7 @@
         <xdr:cNvPr id="43" name="Picture 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8135ECA4-6926-4D9E-84A4-8CFF47F974BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8135ECA4-6926-4D9E-84A4-8CFF47F974BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11796,7 +11818,7 @@
         <xdr:cNvPr id="41" name="Picture 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB5F122D-CEDE-4275-9F1E-149FFDF1E388}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB5F122D-CEDE-4275-9F1E-149FFDF1E388}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11846,7 +11868,7 @@
         <xdr:cNvPr id="46" name="Picture 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FD366AD-6D2A-47C3-8BAD-A5817B6E4052}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9FD366AD-6D2A-47C3-8BAD-A5817B6E4052}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11896,7 +11918,7 @@
         <xdr:cNvPr id="47" name="Picture 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB6D2A6-1AF7-4F21-8948-55E6E89EDD4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEB6D2A6-1AF7-4F21-8948-55E6E89EDD4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11946,7 +11968,7 @@
         <xdr:cNvPr id="45" name="Picture 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268C9EB8-59FE-4E14-B624-F9E0FA8C9A4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{268C9EB8-59FE-4E14-B624-F9E0FA8C9A4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11996,7 +12018,7 @@
         <xdr:cNvPr id="50" name="Picture 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC2E3A4A-21B4-418E-82B8-13DA91685B31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC2E3A4A-21B4-418E-82B8-13DA91685B31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12046,7 +12068,7 @@
         <xdr:cNvPr id="51" name="Picture 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A774D11C-BCC9-4626-A38C-43CDFA0C61A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A774D11C-BCC9-4626-A38C-43CDFA0C61A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12096,7 +12118,7 @@
         <xdr:cNvPr id="49" name="Picture 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3091D98F-39A3-4DED-AB86-11022281925E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3091D98F-39A3-4DED-AB86-11022281925E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12146,7 +12168,7 @@
         <xdr:cNvPr id="54" name="Picture 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D46A7CE-446D-40BD-BAAF-E08CC2916810}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7D46A7CE-446D-40BD-BAAF-E08CC2916810}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12196,7 +12218,7 @@
         <xdr:cNvPr id="55" name="Picture 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE24F44-6FF3-459D-B7B6-61AD5F61515D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8FE24F44-6FF3-459D-B7B6-61AD5F61515D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12246,7 +12268,7 @@
         <xdr:cNvPr id="53" name="Picture 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AFF4CDD-6468-4AC0-9266-9BCA9066048C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AFF4CDD-6468-4AC0-9266-9BCA9066048C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12296,7 +12318,7 @@
         <xdr:cNvPr id="58" name="Picture 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF89DD13-877B-4526-9931-DC1331EB1627}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EF89DD13-877B-4526-9931-DC1331EB1627}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12346,7 +12368,7 @@
         <xdr:cNvPr id="59" name="Picture 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C6BBFBB-3A0D-4F81-8B86-62D335942670}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C6BBFBB-3A0D-4F81-8B86-62D335942670}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12396,7 +12418,7 @@
         <xdr:cNvPr id="57" name="Picture 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AD2DE9-AEBE-4886-BA39-2098C7ACD278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28AD2DE9-AEBE-4886-BA39-2098C7ACD278}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12446,7 +12468,7 @@
         <xdr:cNvPr id="62" name="Picture 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219D88A8-51A3-43CF-91FA-D1C03D6BFC4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{219D88A8-51A3-43CF-91FA-D1C03D6BFC4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12496,7 +12518,7 @@
         <xdr:cNvPr id="63" name="Picture 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C863DD3-89DA-40AE-955B-A207025BBCB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C863DD3-89DA-40AE-955B-A207025BBCB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12546,7 +12568,7 @@
         <xdr:cNvPr id="61" name="Picture 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6532FDD9-9E8C-4CED-BEA1-3588AAAFCD05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6532FDD9-9E8C-4CED-BEA1-3588AAAFCD05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12596,7 +12618,7 @@
         <xdr:cNvPr id="66" name="Picture 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E2A188B-6FFD-484C-B377-17AB21746F5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E2A188B-6FFD-484C-B377-17AB21746F5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12646,7 +12668,7 @@
         <xdr:cNvPr id="67" name="Picture 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0969B6B-28C3-4681-B41E-70E963636C23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0969B6B-28C3-4681-B41E-70E963636C23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12696,7 +12718,7 @@
         <xdr:cNvPr id="65" name="Picture 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA269DB6-46C6-4218-B3C4-C8B01819E87D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA269DB6-46C6-4218-B3C4-C8B01819E87D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12746,7 +12768,7 @@
         <xdr:cNvPr id="70" name="Picture 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B9BA3E-DF82-4DE7-8342-8154C9F1C622}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{62B9BA3E-DF82-4DE7-8342-8154C9F1C622}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12796,7 +12818,7 @@
         <xdr:cNvPr id="71" name="Picture 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89AD693E-AE03-477C-A59D-DA119AD03354}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89AD693E-AE03-477C-A59D-DA119AD03354}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12846,7 +12868,7 @@
         <xdr:cNvPr id="69" name="Picture 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1F82DCD-F711-4055-929C-9039D8C2EE9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1F82DCD-F711-4055-929C-9039D8C2EE9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12896,7 +12918,7 @@
         <xdr:cNvPr id="74" name="Picture 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B045A3C6-F8DF-4129-9198-8F3FD7EFBE62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B045A3C6-F8DF-4129-9198-8F3FD7EFBE62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12946,7 +12968,7 @@
         <xdr:cNvPr id="75" name="Picture 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9055DF6-EFE3-4745-B03C-E512B8030D29}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9055DF6-EFE3-4745-B03C-E512B8030D29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12996,7 +13018,7 @@
         <xdr:cNvPr id="73" name="Picture 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E1E8E5D-9CD8-483B-A965-63B4B8DB4221}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E1E8E5D-9CD8-483B-A965-63B4B8DB4221}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13046,7 +13068,7 @@
         <xdr:cNvPr id="78" name="Picture 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1ED872F-CCCE-40D5-BF89-D47AB08A744C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1ED872F-CCCE-40D5-BF89-D47AB08A744C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13096,7 +13118,7 @@
         <xdr:cNvPr id="79" name="Picture 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA2FB5DC-9F67-45CC-8D0B-5D9411E6E1E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA2FB5DC-9F67-45CC-8D0B-5D9411E6E1E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13146,7 +13168,7 @@
         <xdr:cNvPr id="77" name="Picture 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F9829FD-F645-48AC-8CC3-79FCC46F3623}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F9829FD-F645-48AC-8CC3-79FCC46F3623}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13196,7 +13218,7 @@
         <xdr:cNvPr id="82" name="Picture 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66F63FE7-6012-4746-9787-F455E4CC4AD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66F63FE7-6012-4746-9787-F455E4CC4AD4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13246,7 +13268,7 @@
         <xdr:cNvPr id="83" name="Picture 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2334520F-8F71-49F5-91BB-97D5AFDE78F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2334520F-8F71-49F5-91BB-97D5AFDE78F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13296,7 +13318,7 @@
         <xdr:cNvPr id="81" name="Picture 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B72B181-A6EA-4411-85A3-175E55FA1136}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5B72B181-A6EA-4411-85A3-175E55FA1136}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13346,7 +13368,7 @@
         <xdr:cNvPr id="86" name="Picture 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E829F40-6E2B-4B38-8263-9E03252F0DB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E829F40-6E2B-4B38-8263-9E03252F0DB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13396,7 +13418,7 @@
         <xdr:cNvPr id="87" name="Picture 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9A14DD-2CA3-481B-8F3E-99E6EA13B1A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C9A14DD-2CA3-481B-8F3E-99E6EA13B1A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13446,7 +13468,7 @@
         <xdr:cNvPr id="85" name="Picture 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5513EF9-D185-415D-BA71-860A6E90A43B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5513EF9-D185-415D-BA71-860A6E90A43B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13496,7 +13518,7 @@
         <xdr:cNvPr id="90" name="Picture 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1643AE2-2F85-47C0-B0A1-56EC1E143BDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1643AE2-2F85-47C0-B0A1-56EC1E143BDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13546,7 +13568,7 @@
         <xdr:cNvPr id="91" name="Picture 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7944DA7-71BA-4D41-BE00-6F1BB2CC03F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F7944DA7-71BA-4D41-BE00-6F1BB2CC03F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13596,7 +13618,7 @@
         <xdr:cNvPr id="89" name="Picture 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972BBEE1-94C8-4032-8C1E-43F2698B3B76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{972BBEE1-94C8-4032-8C1E-43F2698B3B76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13646,7 +13668,7 @@
         <xdr:cNvPr id="94" name="Picture 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8954795A-F65C-4D16-958F-24EBDC185FA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8954795A-F65C-4D16-958F-24EBDC185FA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13696,7 +13718,7 @@
         <xdr:cNvPr id="95" name="Picture 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E6624D-C6CE-4279-A0EA-880F00DD7674}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5E6624D-C6CE-4279-A0EA-880F00DD7674}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13746,7 +13768,7 @@
         <xdr:cNvPr id="93" name="Picture 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED8E5D1-9E01-4BB1-AE3A-8F90C342B49A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1ED8E5D1-9E01-4BB1-AE3A-8F90C342B49A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13796,7 +13818,7 @@
         <xdr:cNvPr id="100" name="Picture 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C41B3F25-ED4E-4862-8283-59F4DD2ACB4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C41B3F25-ED4E-4862-8283-59F4DD2ACB4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13846,7 +13868,7 @@
         <xdr:cNvPr id="101" name="Picture 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8305E90C-3ED9-4559-BB6B-4BF7A3A20F5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8305E90C-3ED9-4559-BB6B-4BF7A3A20F5A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13896,7 +13918,7 @@
         <xdr:cNvPr id="97" name="Picture 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{761D5085-AC69-4CED-9A1F-B98E49A1A139}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{761D5085-AC69-4CED-9A1F-B98E49A1A139}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13946,7 +13968,7 @@
         <xdr:cNvPr id="102" name="Picture 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{783D46FA-D932-4677-88DE-22CF7729D355}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{783D46FA-D932-4677-88DE-22CF7729D355}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13996,7 +14018,7 @@
         <xdr:cNvPr id="103" name="Picture 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D835A9-995B-4251-B374-7B0B6EEF235A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7D835A9-995B-4251-B374-7B0B6EEF235A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14046,7 +14068,7 @@
         <xdr:cNvPr id="105" name="Picture 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0AE5A2F-6EE2-4619-B9F1-05C5E8CA3A2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E0AE5A2F-6EE2-4619-B9F1-05C5E8CA3A2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14096,7 +14118,7 @@
         <xdr:cNvPr id="106" name="Picture 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA2D6FCF-9DD4-489B-A17D-802793743362}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA2D6FCF-9DD4-489B-A17D-802793743362}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14146,7 +14168,7 @@
         <xdr:cNvPr id="107" name="Picture 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C059E41-AD5E-41B7-BD6A-26B3047A30FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C059E41-AD5E-41B7-BD6A-26B3047A30FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14196,7 +14218,7 @@
         <xdr:cNvPr id="109" name="Picture 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F1C56CC-E6F1-4BAA-BA4D-5D5606B712F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7F1C56CC-E6F1-4BAA-BA4D-5D5606B712F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14246,7 +14268,7 @@
         <xdr:cNvPr id="110" name="Picture 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E9CDE71-448F-4B48-8B86-03EAE9CD3FFA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0E9CDE71-448F-4B48-8B86-03EAE9CD3FFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14296,7 +14318,7 @@
         <xdr:cNvPr id="111" name="Picture 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B82CD8-BF66-4353-8124-2202FB70422F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77B82CD8-BF66-4353-8124-2202FB70422F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14346,7 +14368,7 @@
         <xdr:cNvPr id="113" name="Picture 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03236BD3-06FA-44C5-B296-D2749AA0D2F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{03236BD3-06FA-44C5-B296-D2749AA0D2F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14396,7 +14418,7 @@
         <xdr:cNvPr id="114" name="Picture 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9F07DDD-DA56-44A9-BFF5-25506DA09DEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9F07DDD-DA56-44A9-BFF5-25506DA09DEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14446,7 +14468,7 @@
         <xdr:cNvPr id="115" name="Picture 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D075DCC8-DF72-4DA8-8E05-A7E4524E641B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D075DCC8-DF72-4DA8-8E05-A7E4524E641B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14496,7 +14518,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{386EDEDB-C790-4B9C-B601-30D65C127308}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{386EDEDB-C790-4B9C-B601-30D65C127308}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14546,7 +14568,7 @@
         <xdr:cNvPr id="88" name="Picture 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC212AEE-0C98-44DE-A5C2-921C49961C9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC212AEE-0C98-44DE-A5C2-921C49961C9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14596,7 +14618,7 @@
         <xdr:cNvPr id="92" name="Picture 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118DACD7-BAFA-4CC4-9694-CFD014FE8AE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118DACD7-BAFA-4CC4-9694-CFD014FE8AE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14646,7 +14668,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{204C9863-1D5F-4EF0-88D3-D28A0BD9643E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{204C9863-1D5F-4EF0-88D3-D28A0BD9643E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14696,7 +14718,7 @@
         <xdr:cNvPr id="96" name="Picture 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA29762E-6A19-4AF6-B954-D683CEE32E22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EA29762E-6A19-4AF6-B954-D683CEE32E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14746,7 +14768,7 @@
         <xdr:cNvPr id="98" name="Picture 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D16448A-B33C-4535-8A78-36B0E518B16A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0D16448A-B33C-4535-8A78-36B0E518B16A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14796,7 +14818,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18FBDACA-08EA-4786-B95D-5EA28C84BFB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18FBDACA-08EA-4786-B95D-5EA28C84BFB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14846,7 +14868,7 @@
         <xdr:cNvPr id="99" name="Picture 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC79F0CD-E530-4D2C-9A0E-6EFD551E0745}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC79F0CD-E530-4D2C-9A0E-6EFD551E0745}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14896,7 +14918,7 @@
         <xdr:cNvPr id="104" name="Picture 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A06AE1-0FFC-4194-945D-A65E9964C0A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6A06AE1-0FFC-4194-945D-A65E9964C0A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14946,7 +14968,7 @@
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7E6438-16FE-436E-B3C5-23BC6D391157}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D7E6438-16FE-436E-B3C5-23BC6D391157}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14996,7 +15018,7 @@
         <xdr:cNvPr id="108" name="Picture 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E7E415-E395-4BC5-A843-328CE5C012D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55E7E415-E395-4BC5-A843-328CE5C012D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15046,7 +15068,7 @@
         <xdr:cNvPr id="112" name="Picture 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40246C0-BC20-4BC1-9884-A07D67C7AB97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A40246C0-BC20-4BC1-9884-A07D67C7AB97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15124,7 +15146,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -15176,7 +15198,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -15370,14 +15392,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7841E7F-AE8F-44BD-B850-8391483B98A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15387,12 +15409,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43">
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
@@ -15523,7 +15545,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43">
       <c r="A2" s="81" t="s">
         <v>2079</v>
       </c>
@@ -15654,7 +15676,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43">
       <c r="A3" s="81" t="s">
         <v>44</v>
       </c>
@@ -15785,7 +15807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43">
       <c r="A4" s="81" t="s">
         <v>86</v>
       </c>
@@ -15916,7 +15938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43">
       <c r="A5" s="81" t="s">
         <v>129</v>
       </c>
@@ -16047,7 +16069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43">
       <c r="A6" s="81" t="s">
         <v>170</v>
       </c>
@@ -16178,7 +16200,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43">
       <c r="A7" s="81" t="s">
         <v>209</v>
       </c>
@@ -16309,7 +16331,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43">
       <c r="A8" s="81" t="s">
         <v>251</v>
       </c>
@@ -16440,7 +16462,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43">
       <c r="A9" s="81" t="s">
         <v>276</v>
       </c>
@@ -16571,7 +16593,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43">
       <c r="A10" s="81" t="s">
         <v>306</v>
       </c>
@@ -16702,7 +16724,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43">
       <c r="A11" s="81" t="s">
         <v>337</v>
       </c>
@@ -16833,7 +16855,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43">
       <c r="A12" s="81" t="s">
         <v>361</v>
       </c>
@@ -16964,7 +16986,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43">
       <c r="A13" s="81" t="s">
         <v>307</v>
       </c>
@@ -17095,7 +17117,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43">
       <c r="A14" s="81" t="s">
         <v>401</v>
       </c>
@@ -17226,7 +17248,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43">
       <c r="A15" s="81" t="s">
         <v>441</v>
       </c>
@@ -17357,7 +17379,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18" s="81" t="s">
         <v>470</v>
       </c>
@@ -17488,7 +17510,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19" s="81" t="s">
         <v>501</v>
       </c>
@@ -17619,7 +17641,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20" s="81" t="s">
         <v>533</v>
       </c>
@@ -17750,7 +17772,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21" s="81" t="s">
         <v>567</v>
       </c>
@@ -17881,7 +17903,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22" s="81" t="s">
         <v>601</v>
       </c>
@@ -18012,7 +18034,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23" s="81" t="s">
         <v>635</v>
       </c>
@@ -18143,7 +18165,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24" s="81" t="s">
         <v>668</v>
       </c>
@@ -18274,7 +18296,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25" s="81" t="s">
         <v>700</v>
       </c>
@@ -18405,7 +18427,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26" s="81" t="s">
         <v>726</v>
       </c>
@@ -18536,7 +18558,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27" s="81" t="s">
         <v>534</v>
       </c>
@@ -18667,7 +18689,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28" s="81" t="s">
         <v>770</v>
       </c>
@@ -18798,7 +18820,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29" s="81" t="s">
         <v>794</v>
       </c>
@@ -18929,7 +18951,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30" s="81" t="s">
         <v>819</v>
       </c>
@@ -19060,7 +19082,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31" s="81" t="s">
         <v>848</v>
       </c>
@@ -19191,7 +19213,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32" s="81" t="s">
         <v>876</v>
       </c>
@@ -19322,7 +19344,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33" s="81" t="s">
         <v>903</v>
       </c>
@@ -19453,7 +19475,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34" s="81" t="s">
         <v>928</v>
       </c>
@@ -19584,7 +19606,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35" s="81" t="s">
         <v>952</v>
       </c>
@@ -19715,7 +19737,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36" s="81" t="s">
         <v>977</v>
       </c>
@@ -19846,7 +19868,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37" s="81" t="s">
         <v>1004</v>
       </c>
@@ -19977,7 +19999,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38" s="81" t="s">
         <v>1039</v>
       </c>
@@ -20108,7 +20130,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39" s="81" t="s">
         <v>1076</v>
       </c>
@@ -20239,7 +20261,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43">
       <c r="A40" s="81" t="s">
         <v>1101</v>
       </c>
@@ -20370,7 +20392,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43">
       <c r="A41" s="81" t="s">
         <v>1122</v>
       </c>
@@ -20501,7 +20523,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43">
       <c r="A42" s="81" t="s">
         <v>1153</v>
       </c>
@@ -20632,7 +20654,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43">
       <c r="A43" s="81" t="s">
         <v>1174</v>
       </c>
@@ -20763,7 +20785,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43">
       <c r="A44" s="81" t="s">
         <v>1197</v>
       </c>
@@ -20894,7 +20916,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43">
       <c r="A45" s="81" t="s">
         <v>2178</v>
       </c>
@@ -21025,7 +21047,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43">
       <c r="A46" s="81" t="s">
         <v>1235</v>
       </c>
@@ -21156,7 +21178,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43">
       <c r="A47" s="81" t="s">
         <v>2174</v>
       </c>
@@ -21287,7 +21309,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43">
       <c r="A48" s="81" t="s">
         <v>2171</v>
       </c>
@@ -21418,7 +21440,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43">
       <c r="A49" s="81" t="s">
         <v>1266</v>
       </c>
@@ -21549,7 +21571,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43">
       <c r="A50" s="81" t="s">
         <v>1297</v>
       </c>
@@ -21680,7 +21702,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43">
       <c r="A51" s="81" t="s">
         <v>1333</v>
       </c>
@@ -21811,7 +21833,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43">
       <c r="A52" s="81" t="s">
         <v>1363</v>
       </c>
@@ -21942,7 +21964,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43">
       <c r="A53" s="81" t="s">
         <v>2172</v>
       </c>
@@ -22073,7 +22095,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43">
       <c r="A54" s="81" t="s">
         <v>2175</v>
       </c>
@@ -22204,7 +22226,7 @@
         <v>2353</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43">
       <c r="A55" s="81" t="s">
         <v>1389</v>
       </c>
@@ -22335,7 +22357,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43">
       <c r="A56" s="81" t="s">
         <v>1411</v>
       </c>
@@ -22466,7 +22488,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43">
       <c r="A57" s="81" t="s">
         <v>2173</v>
       </c>
@@ -22597,7 +22619,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43">
       <c r="A58" s="81" t="s">
         <v>2179</v>
       </c>
@@ -22728,7 +22750,7 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43">
       <c r="A59" s="81" t="s">
         <v>2177</v>
       </c>
@@ -22859,7 +22881,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43">
       <c r="A60" s="81" t="s">
         <v>2169</v>
       </c>
@@ -22990,7 +23012,7 @@
         <v>2456</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43">
       <c r="A61" s="81" t="s">
         <v>1440</v>
       </c>
@@ -23121,7 +23143,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43">
       <c r="A62" s="81" t="s">
         <v>1459</v>
       </c>
@@ -23252,7 +23274,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43">
       <c r="A63" s="81" t="s">
         <v>1489</v>
       </c>
@@ -23383,7 +23405,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43">
       <c r="A64" s="81" t="s">
         <v>2170</v>
       </c>
@@ -23514,7 +23536,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43">
       <c r="A65" s="81" t="s">
         <v>1519</v>
       </c>
@@ -23645,7 +23667,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43">
       <c r="A66" s="81" t="s">
         <v>1544</v>
       </c>
@@ -23776,7 +23798,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43">
       <c r="A67" s="81" t="s">
         <v>1580</v>
       </c>
@@ -23907,7 +23929,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43">
       <c r="A68" s="81" t="s">
         <v>2176</v>
       </c>
@@ -24038,7 +24060,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43">
       <c r="A69" s="81" t="s">
         <v>2168</v>
       </c>
@@ -24169,7 +24191,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43">
       <c r="A70" s="81" t="s">
         <v>1617</v>
       </c>
@@ -24300,7 +24322,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43">
       <c r="A71" s="81" t="s">
         <v>1623</v>
       </c>
@@ -24431,7 +24453,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43">
       <c r="A72" s="81" t="s">
         <v>1629</v>
       </c>
@@ -24562,7 +24584,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43">
       <c r="A73" s="81" t="s">
         <v>1635</v>
       </c>
@@ -24693,7 +24715,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43">
       <c r="A74" s="81" t="s">
         <v>1641</v>
       </c>
@@ -24824,7 +24846,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43">
       <c r="A75" s="81" t="s">
         <v>1649</v>
       </c>
@@ -24955,7 +24977,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43">
       <c r="A76" s="81" t="s">
         <v>1657</v>
       </c>
@@ -25086,7 +25108,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43">
       <c r="A77" s="81" t="s">
         <v>1664</v>
       </c>
@@ -25217,7 +25239,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43">
       <c r="A78" s="81" t="s">
         <v>1671</v>
       </c>
@@ -25348,7 +25370,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43">
       <c r="A79" s="81" t="s">
         <v>1678</v>
       </c>
@@ -25479,7 +25501,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43">
       <c r="A80" s="81" t="s">
         <v>1685</v>
       </c>
@@ -25610,7 +25632,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43">
       <c r="A81" s="81" t="s">
         <v>1692</v>
       </c>
@@ -25741,7 +25763,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43">
       <c r="A82" s="81" t="s">
         <v>1699</v>
       </c>
@@ -25872,7 +25894,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43">
       <c r="A83" s="81" t="s">
         <v>1707</v>
       </c>
@@ -26003,7 +26025,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43">
       <c r="A84" s="81" t="s">
         <v>1715</v>
       </c>
@@ -26134,7 +26156,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43">
       <c r="A85" s="81" t="s">
         <v>1722</v>
       </c>
@@ -26265,7 +26287,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43">
       <c r="A86" s="81" t="s">
         <v>1728</v>
       </c>
@@ -26396,7 +26418,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43">
       <c r="A87" s="81" t="s">
         <v>1748</v>
       </c>
@@ -26527,7 +26549,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:43">
       <c r="A88" s="81" t="s">
         <v>1768</v>
       </c>
@@ -26658,7 +26680,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43">
       <c r="A89" s="81" t="s">
         <v>1788</v>
       </c>
@@ -26789,7 +26811,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43">
       <c r="A90" s="81" t="s">
         <v>1808</v>
       </c>
@@ -26920,7 +26942,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43">
       <c r="A91" s="81" t="s">
         <v>1828</v>
       </c>
@@ -27051,7 +27073,7 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43">
       <c r="A92" s="81" t="s">
         <v>1848</v>
       </c>
@@ -27182,7 +27204,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43">
       <c r="A93" s="81" t="s">
         <v>1868</v>
       </c>
@@ -27313,7 +27335,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43">
       <c r="A94" s="81" t="s">
         <v>1888</v>
       </c>
@@ -27444,7 +27466,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43">
       <c r="A95" s="81" t="s">
         <v>1908</v>
       </c>
@@ -27575,7 +27597,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43">
       <c r="A96" s="81" t="s">
         <v>1928</v>
       </c>
@@ -27706,7 +27728,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43">
       <c r="A97" s="81" t="s">
         <v>1948</v>
       </c>
@@ -27837,7 +27859,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43">
       <c r="A98" s="81" t="s">
         <v>1968</v>
       </c>
@@ -27968,7 +27990,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43">
       <c r="A99" s="81" t="s">
         <v>1988</v>
       </c>
@@ -28099,7 +28121,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43">
       <c r="A100" s="81" t="s">
         <v>1978</v>
       </c>
@@ -28230,7 +28252,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43">
       <c r="A101" s="81" t="s">
         <v>1998</v>
       </c>
@@ -28361,7 +28383,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43">
       <c r="A102" s="81" t="s">
         <v>2192</v>
       </c>
@@ -28492,43 +28514,43 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:43">
       <c r="A103" s="82"/>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43">
       <c r="A104" s="82"/>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:43">
       <c r="A105" s="82"/>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43">
       <c r="A106" s="82"/>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43">
       <c r="A107" s="82"/>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43">
       <c r="A108" s="82"/>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43">
       <c r="A109" s="82"/>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43">
       <c r="A110" s="82"/>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43">
       <c r="A111" s="82"/>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43">
       <c r="A112" s="82"/>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:42">
       <c r="A113" s="82"/>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:42">
       <c r="A114" s="82"/>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:42">
       <c r="A115" s="81" t="s">
         <v>2037</v>
       </c>
@@ -28658,34 +28680,39 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6F2527-19E5-4875-93D2-CFC0AC718D02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="11"/>
-    <col min="5" max="5" width="1.140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="11"/>
-    <col min="7" max="7" width="27.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="1.140625" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="1.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="11"/>
+    <col min="5" max="5" width="1.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="11"/>
+    <col min="7" max="7" width="27.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="7.5" customHeight="1"/>
+    <row r="2" spans="2:9" ht="16" thickBot="1">
       <c r="B2" s="83" t="s">
         <v>2121</v>
       </c>
@@ -28697,7 +28724,7 @@
       <c r="G2" s="84"/>
       <c r="H2" s="85"/>
     </row>
-    <row r="3" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="9" customHeight="1">
       <c r="B3" s="86"/>
       <c r="C3" s="87"/>
       <c r="D3" s="88"/>
@@ -28705,7 +28732,7 @@
       <c r="G3" s="87"/>
       <c r="H3" s="88"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="98" t="s">
         <v>2123</v>
       </c>
@@ -28717,7 +28744,7 @@
       <c r="G4" s="89"/>
       <c r="H4" s="88"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" s="86"/>
       <c r="C5" s="87"/>
       <c r="D5" s="88"/>
@@ -28729,7 +28756,7 @@
       </c>
       <c r="H5" s="88"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="98" t="s">
         <v>2126</v>
       </c>
@@ -28745,7 +28772,7 @@
       </c>
       <c r="H6" s="88"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="86"/>
       <c r="C7" s="87"/>
       <c r="D7" s="88"/>
@@ -28757,7 +28784,7 @@
       </c>
       <c r="H7" s="88"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="98" t="s">
         <v>2131</v>
       </c>
@@ -28773,7 +28800,7 @@
       </c>
       <c r="H8" s="88"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" s="86"/>
       <c r="C9" s="87"/>
       <c r="D9" s="88"/>
@@ -28785,7 +28812,7 @@
       </c>
       <c r="H9" s="88"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="98" t="s">
         <v>2137</v>
       </c>
@@ -28797,7 +28824,7 @@
       <c r="G10" s="94"/>
       <c r="H10" s="88"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" s="86"/>
       <c r="C11" s="87"/>
       <c r="D11" s="88"/>
@@ -28805,7 +28832,7 @@
       <c r="G11" s="96"/>
       <c r="H11" s="97"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="98" t="s">
         <v>2191</v>
       </c>
@@ -28814,13 +28841,13 @@
       </c>
       <c r="D12" s="88"/>
     </row>
-    <row r="13" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="9" customHeight="1">
       <c r="B13" s="95"/>
       <c r="C13" s="96"/>
       <c r="D13" s="97"/>
     </row>
-    <row r="14" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="9" customHeight="1"/>
+    <row r="15" spans="2:9" ht="9" customHeight="1">
       <c r="B15" s="99"/>
       <c r="C15" s="100"/>
       <c r="D15" s="101"/>
@@ -28837,7 +28864,7 @@
         <v>Argentina</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="16" thickBot="1">
       <c r="B16" s="86"/>
       <c r="C16" s="102" t="s">
         <v>2136</v>
@@ -28853,7 +28880,7 @@
       <c r="H16" s="108"/>
       <c r="I16" s="108"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9">
       <c r="B17" s="103" t="str">
         <f>VLOOKUP("Germany",T,lang,FALSE)</f>
         <v>Germany</v>
@@ -28869,7 +28896,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" s="103" t="str">
         <f>VLOOKUP("Brazil",T,lang,FALSE)</f>
         <v>Brazil</v>
@@ -28889,7 +28916,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9">
       <c r="B19" s="103" t="str">
         <f>VLOOKUP("Portugal",T,lang,FALSE)</f>
         <v>Portugal</v>
@@ -28909,7 +28936,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" s="103" t="str">
         <f>VLOOKUP("Argentina",T,lang,FALSE)</f>
         <v>Argentina</v>
@@ -28929,7 +28956,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" s="103" t="str">
         <f>VLOOKUP("Belgium",T,lang,FALSE)</f>
         <v>Belgium</v>
@@ -28949,7 +28976,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9">
       <c r="B22" s="103" t="str">
         <f>VLOOKUP("Spain",T,lang,FALSE)</f>
         <v>Spain</v>
@@ -28969,7 +28996,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9">
       <c r="B23" s="103" t="str">
         <f>VLOOKUP("Poland",T,lang,FALSE)</f>
         <v>Poland</v>
@@ -28989,7 +29016,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9">
       <c r="B24" s="103" t="str">
         <f>VLOOKUP("Switzerland",T,lang,FALSE)</f>
         <v>Switzerland</v>
@@ -29009,7 +29036,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9">
       <c r="B25" s="103" t="str">
         <f>VLOOKUP("France",T,lang,FALSE)</f>
         <v>France</v>
@@ -29029,7 +29056,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9">
       <c r="B26" s="103" t="str">
         <f>VLOOKUP("Peru",T,lang,FALSE)</f>
         <v>Peru</v>
@@ -29049,7 +29076,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9">
       <c r="B27" s="103" t="str">
         <f>VLOOKUP("Denmark",T,lang,FALSE)</f>
         <v>Denmark</v>
@@ -29069,7 +29096,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" s="103" t="str">
         <f>VLOOKUP("Colombia",T,lang,FALSE)</f>
         <v>Colombia</v>
@@ -29089,7 +29116,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9">
       <c r="B29" s="103" t="str">
         <f>VLOOKUP("England",T,lang,FALSE)</f>
         <v>England</v>
@@ -29109,7 +29136,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9">
       <c r="B30" s="103" t="str">
         <f>VLOOKUP("Mexico",T,lang,FALSE)</f>
         <v>Mexico</v>
@@ -29129,7 +29156,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9">
       <c r="B31" s="103" t="str">
         <f>VLOOKUP("Croatia",T,lang,FALSE)</f>
         <v>Croatia</v>
@@ -29149,7 +29176,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9">
       <c r="B32" s="103" t="str">
         <f>VLOOKUP("Sweden",T,lang,FALSE)</f>
         <v>Sweden</v>
@@ -29169,7 +29196,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9">
       <c r="B33" s="103" t="str">
         <f>VLOOKUP("Uruguay",T,lang,FALSE)</f>
         <v>Uruguay</v>
@@ -29189,7 +29216,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" s="103" t="str">
         <f>VLOOKUP("Iceland",T,lang,FALSE)</f>
         <v>Iceland</v>
@@ -29209,7 +29236,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="103" t="str">
         <f>VLOOKUP("Senegal",T,lang,FALSE)</f>
         <v>Senegal</v>
@@ -29229,7 +29256,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="103" t="str">
         <f>VLOOKUP("Costa Rica",T,lang,FALSE)</f>
         <v>Costa Rica</v>
@@ -29249,7 +29276,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="103" t="str">
         <f>VLOOKUP("Tunisia",T,lang,FALSE)</f>
         <v>Tunisia</v>
@@ -29269,7 +29296,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="103" t="str">
         <f>VLOOKUP("Egypt",T,lang,FALSE)</f>
         <v>Egypt</v>
@@ -29289,7 +29316,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="103" t="str">
         <f>VLOOKUP("Iran",T,lang,FALSE)</f>
         <v>Iran</v>
@@ -29309,7 +29336,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="103" t="str">
         <f>VLOOKUP("Serbia",T,lang,FALSE)</f>
         <v>Serbia</v>
@@ -29329,7 +29356,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="103" t="str">
         <f>VLOOKUP("Australia",T,lang,FALSE)</f>
         <v>Australia</v>
@@ -29349,7 +29376,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="103" t="str">
         <f>VLOOKUP("Morocco",T,lang,FALSE)</f>
         <v>Morocco</v>
@@ -29365,7 +29392,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9">
       <c r="B43" s="103" t="str">
         <f>VLOOKUP("Nigeria",T,lang,FALSE)</f>
         <v>Nigeria</v>
@@ -29385,7 +29412,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="103" t="str">
         <f>VLOOKUP("Panama",T,lang,FALSE)</f>
         <v>Panama</v>
@@ -29405,7 +29432,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="B45" s="103" t="str">
         <f>VLOOKUP("Japan",T,lang,FALSE)</f>
         <v>Japan</v>
@@ -29425,7 +29452,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9">
       <c r="B46" s="103" t="str">
         <f>VLOOKUP("Korea Republic",T,lang,FALSE)</f>
         <v>Korea Republic</v>
@@ -29445,7 +29472,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9">
       <c r="B47" s="103" t="str">
         <f>VLOOKUP("Saudi Arabia",T,lang,FALSE)</f>
         <v>Saudi Arabia</v>
@@ -29461,7 +29488,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9">
       <c r="B48" s="103" t="str">
         <f>VLOOKUP("Russia",T,lang,FALSE)</f>
         <v>Russia</v>
@@ -29482,7 +29509,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4">
       <c r="B49" s="95"/>
       <c r="C49" s="96"/>
       <c r="D49" s="97"/>
@@ -29493,109 +29520,114 @@
     <sortCondition ref="I17:I48"/>
   </sortState>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Language" prompt="Use drop-down List" sqref="C4" xr:uid="{0DBAD2C3-6A5E-43E5-9FC6-9E3CAE1C968A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Language" prompt="Use drop-down List" sqref="C4">
       <formula1>lang_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Summer Time" prompt="Use drop-down List" sqref="C6" xr:uid="{28AC6A07-581B-484E-B93A-3F6462423AE7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Summer Time" prompt="Use drop-down List" sqref="C6">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select GTM-time" prompt="Use drop-down List" sqref="C8" xr:uid="{EC83C832-B212-425C-9943-F17313271E59}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select GTM-time" prompt="Use drop-down List" sqref="C8">
       <formula1>$F$18:$F$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Minutes" prompt="Use drop-down List" sqref="C10" xr:uid="{C6794E40-584C-4822-8504-C53404E82E2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Minutes" prompt="Use drop-down List" sqref="C10">
       <formula1>$F$43:$F$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Your Favorite Team" prompt="Use drop-down List" sqref="C12" xr:uid="{5F5DA096-193C-403D-9698-1DEED542F9BD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Your Favorite Team" prompt="Use drop-down List" sqref="C12">
       <formula1>teams</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFCDAAD0-B7F9-4EC8-A89D-FA373AF4B5F2}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BT97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="6" customWidth="1"/>
-    <col min="6" max="7" width="4.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="6" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="8" customWidth="1"/>
+    <col min="9" max="9" width="3.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="14" style="9" customWidth="1"/>
-    <col min="11" max="14" width="5.42578125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="10" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" style="10" customWidth="1"/>
-    <col min="17" max="17" width="3.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="58" hidden="1" customWidth="1"/>
+    <col min="11" max="14" width="5.5" style="10" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="2" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="58" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="16" style="65" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="5" style="59" hidden="1" customWidth="1"/>
-    <col min="22" max="25" width="6.140625" style="58" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="4.28515625" style="59" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="5.42578125" style="58" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="13.42578125" style="59" hidden="1" customWidth="1"/>
-    <col min="29" max="33" width="5.42578125" style="58" hidden="1" customWidth="1"/>
+    <col min="22" max="25" width="6.1640625" style="58" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="4.33203125" style="59" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5" style="58" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5" style="59" hidden="1" customWidth="1"/>
+    <col min="29" max="33" width="5.5" style="58" hidden="1" customWidth="1"/>
     <col min="34" max="36" width="6" style="58" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="5.42578125" style="58" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="5.5" style="58" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="6" style="58" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="7.140625" style="59" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="7.1640625" style="59" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="10" style="59" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="15.28515625" style="60" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="4.7109375" style="61" hidden="1" customWidth="1"/>
-    <col min="43" max="46" width="4.7109375" style="62" hidden="1" customWidth="1"/>
-    <col min="47" max="49" width="9.140625" style="63" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="9.140625" style="64" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="3.28515625" style="3" customWidth="1"/>
-    <col min="52" max="52" width="19.7109375" style="3" customWidth="1"/>
+    <col min="41" max="41" width="15.33203125" style="60" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="4.6640625" style="61" hidden="1" customWidth="1"/>
+    <col min="43" max="46" width="4.6640625" style="62" hidden="1" customWidth="1"/>
+    <col min="47" max="49" width="9.1640625" style="63" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="9.1640625" style="64" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="3.33203125" style="3" customWidth="1"/>
+    <col min="52" max="52" width="19.6640625" style="3" customWidth="1"/>
     <col min="53" max="54" width="3" style="3" customWidth="1"/>
     <col min="55" max="56" width="2" style="3" customWidth="1"/>
-    <col min="57" max="57" width="3.28515625" style="3" customWidth="1"/>
-    <col min="58" max="58" width="19.7109375" style="3" customWidth="1"/>
+    <col min="57" max="57" width="3.33203125" style="3" customWidth="1"/>
+    <col min="58" max="58" width="19.6640625" style="3" customWidth="1"/>
     <col min="59" max="60" width="3" style="3" customWidth="1"/>
     <col min="61" max="62" width="2" style="3" customWidth="1"/>
-    <col min="63" max="63" width="3.28515625" style="3" customWidth="1"/>
-    <col min="64" max="64" width="19.7109375" style="3" customWidth="1"/>
+    <col min="63" max="63" width="3.33203125" style="3" customWidth="1"/>
+    <col min="64" max="64" width="19.6640625" style="3" customWidth="1"/>
     <col min="65" max="66" width="3" style="3" customWidth="1"/>
     <col min="67" max="68" width="2" style="3" customWidth="1"/>
-    <col min="69" max="69" width="3.28515625" style="3" customWidth="1"/>
-    <col min="70" max="70" width="19.7109375" style="3" customWidth="1"/>
+    <col min="69" max="69" width="3.33203125" style="3" customWidth="1"/>
+    <col min="70" max="70" width="19.6640625" style="3" customWidth="1"/>
     <col min="71" max="72" width="3" style="3" customWidth="1"/>
-    <col min="73" max="16384" width="9.140625" style="3"/>
+    <col min="73" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="str">
+    <row r="1" spans="1:72" ht="45">
+      <c r="A1" s="115" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
       <c r="U1" s="58"/>
@@ -29619,7 +29651,7 @@
       <c r="AS1" s="63"/>
       <c r="AT1" s="63"/>
     </row>
-    <row r="2" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" ht="3" customHeight="1">
       <c r="S2" s="58"/>
       <c r="T2" s="58"/>
       <c r="U2" s="58"/>
@@ -29643,7 +29675,7 @@
       <c r="AS2" s="63"/>
       <c r="AT2" s="63"/>
     </row>
-    <row r="3" spans="1:72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" ht="12.75" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -29658,11 +29690,11 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="116" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="116"/>
       <c r="S3" s="58"/>
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
@@ -29686,45 +29718,45 @@
       <c r="AS3" s="63"/>
       <c r="AT3" s="63"/>
     </row>
-    <row r="4" spans="1:72" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="138" t="str">
+    <row r="4" spans="1:72" ht="3" customHeight="1"/>
+    <row r="5" spans="1:72" ht="15" customHeight="1">
+      <c r="A5" s="117" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
+      <c r="J5" s="123" t="s">
         <v>2181</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="125"/>
     </row>
-    <row r="6" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+    <row r="6" spans="1:72" ht="15" customHeight="1">
+      <c r="A6" s="120"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="128"/>
       <c r="R6" s="58" t="s">
         <v>2182</v>
       </c>
@@ -29788,36 +29820,36 @@
       <c r="AT6" s="62" t="s">
         <v>2189</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="109" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="AZ6" s="131"/>
-      <c r="BA6" s="131"/>
-      <c r="BB6" s="132"/>
-      <c r="BE6" s="130" t="str">
+      <c r="AZ6" s="110"/>
+      <c r="BA6" s="110"/>
+      <c r="BB6" s="111"/>
+      <c r="BE6" s="109" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BF6" s="131"/>
-      <c r="BG6" s="131"/>
-      <c r="BH6" s="132"/>
-      <c r="BK6" s="130" t="str">
+      <c r="BF6" s="110"/>
+      <c r="BG6" s="110"/>
+      <c r="BH6" s="111"/>
+      <c r="BK6" s="109" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="131"/>
-      <c r="BN6" s="132"/>
-      <c r="BQ6" s="130" t="str">
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="110"/>
+      <c r="BN6" s="111"/>
+      <c r="BQ6" s="109" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
+      <c r="BR6" s="110"/>
+      <c r="BS6" s="110"/>
+      <c r="BT6" s="111"/>
     </row>
-    <row r="7" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" ht="15" customHeight="1">
       <c r="A7" s="12">
         <v>1</v>
       </c>
@@ -29875,24 +29907,24 @@
         <f>IF(OR(F7="",G7=""),"",IF(F7&gt;G7,1,IF(F7&lt;G7,-1,0)))</f>
         <v/>
       </c>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="134"/>
-      <c r="BA7" s="134"/>
-      <c r="BB7" s="135"/>
-      <c r="BE7" s="133"/>
-      <c r="BF7" s="134"/>
-      <c r="BG7" s="134"/>
-      <c r="BH7" s="135"/>
-      <c r="BK7" s="133"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="134"/>
-      <c r="BN7" s="135"/>
-      <c r="BQ7" s="133"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
+      <c r="AY7" s="112"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="114"/>
+      <c r="BE7" s="112"/>
+      <c r="BF7" s="113"/>
+      <c r="BG7" s="113"/>
+      <c r="BH7" s="114"/>
+      <c r="BK7" s="112"/>
+      <c r="BL7" s="113"/>
+      <c r="BM7" s="113"/>
+      <c r="BN7" s="114"/>
+      <c r="BQ7" s="112"/>
+      <c r="BR7" s="113"/>
+      <c r="BS7" s="113"/>
+      <c r="BT7" s="114"/>
     </row>
-    <row r="8" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" ht="15" customHeight="1">
       <c r="A8" s="18">
         <v>2</v>
       </c>
@@ -30070,7 +30102,7 @@
       <c r="BS8" s="25"/>
       <c r="BT8" s="25"/>
     </row>
-    <row r="9" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" ht="15" customHeight="1">
       <c r="A9" s="18">
         <v>3</v>
       </c>
@@ -30262,7 +30294,7 @@
       <c r="BS9" s="25"/>
       <c r="BT9" s="25"/>
     </row>
-    <row r="10" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" ht="15" customHeight="1">
       <c r="A10" s="18">
         <v>4</v>
       </c>
@@ -30424,7 +30456,7 @@
         <f>AR10-AS10</f>
         <v>0</v>
       </c>
-      <c r="AY10" s="118">
+      <c r="AY10" s="129">
         <v>49</v>
       </c>
       <c r="AZ10" s="28" t="str">
@@ -30452,7 +30484,7 @@
       <c r="BS10" s="25"/>
       <c r="BT10" s="25"/>
     </row>
-    <row r="11" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" ht="15" customHeight="1">
       <c r="A11" s="18">
         <v>5</v>
       </c>
@@ -30614,7 +30646,7 @@
         <f>AR11-AS11</f>
         <v>0</v>
       </c>
-      <c r="AY11" s="119"/>
+      <c r="AY11" s="130"/>
       <c r="AZ11" s="31" t="str">
         <f>AO15</f>
         <v>2B</v>
@@ -30643,7 +30675,7 @@
       <c r="BS11" s="25"/>
       <c r="BT11" s="25"/>
     </row>
-    <row r="12" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" ht="15" customHeight="1">
       <c r="A12" s="18">
         <v>6</v>
       </c>
@@ -30791,7 +30823,7 @@
       <c r="BB12" s="25"/>
       <c r="BC12" s="36"/>
       <c r="BD12" s="25"/>
-      <c r="BE12" s="118">
+      <c r="BE12" s="129">
         <v>57</v>
       </c>
       <c r="BF12" s="28" t="str">
@@ -30813,7 +30845,7 @@
       <c r="BS12" s="25"/>
       <c r="BT12" s="25"/>
     </row>
-    <row r="13" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" ht="15" customHeight="1">
       <c r="A13" s="18">
         <v>7</v>
       </c>
@@ -30895,7 +30927,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="36"/>
       <c r="BD13" s="39"/>
-      <c r="BE13" s="119"/>
+      <c r="BE13" s="130"/>
       <c r="BF13" s="31" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -30915,7 +30947,7 @@
       <c r="BS13" s="25"/>
       <c r="BT13" s="25"/>
     </row>
-    <row r="14" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" ht="15" customHeight="1">
       <c r="A14" s="18">
         <v>8</v>
       </c>
@@ -31081,7 +31113,7 @@
         <f>AR14-AS14</f>
         <v>0</v>
       </c>
-      <c r="AY14" s="118">
+      <c r="AY14" s="129">
         <v>50</v>
       </c>
       <c r="AZ14" s="28" t="str">
@@ -31109,7 +31141,7 @@
       <c r="BS14" s="25"/>
       <c r="BT14" s="25"/>
     </row>
-    <row r="15" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" ht="15" customHeight="1">
       <c r="A15" s="18">
         <v>9</v>
       </c>
@@ -31275,7 +31307,7 @@
         <f>AR15-AS15</f>
         <v>0</v>
       </c>
-      <c r="AY15" s="119"/>
+      <c r="AY15" s="130"/>
       <c r="AZ15" s="31" t="str">
         <f>AO27</f>
         <v>2D</v>
@@ -31304,7 +31336,7 @@
       <c r="BS15" s="25"/>
       <c r="BT15" s="25"/>
     </row>
-    <row r="16" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" ht="15" customHeight="1">
       <c r="A16" s="18">
         <v>10</v>
       </c>
@@ -31478,7 +31510,7 @@
       <c r="BH16" s="25"/>
       <c r="BI16" s="36"/>
       <c r="BJ16" s="25"/>
-      <c r="BK16" s="118">
+      <c r="BK16" s="129">
         <v>61</v>
       </c>
       <c r="BL16" s="28" t="str">
@@ -31494,7 +31526,7 @@
       <c r="BS16" s="25"/>
       <c r="BT16" s="25"/>
     </row>
-    <row r="17" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72" ht="15" customHeight="1">
       <c r="A17" s="18">
         <v>11</v>
       </c>
@@ -31671,7 +31703,7 @@
       <c r="BH17" s="25"/>
       <c r="BI17" s="36"/>
       <c r="BJ17" s="39"/>
-      <c r="BK17" s="119"/>
+      <c r="BK17" s="130"/>
       <c r="BL17" s="31" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -31685,7 +31717,7 @@
       <c r="BS17" s="25"/>
       <c r="BT17" s="25"/>
     </row>
-    <row r="18" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72" ht="15" customHeight="1">
       <c r="A18" s="18">
         <v>12</v>
       </c>
@@ -31827,7 +31859,7 @@
         <f>MAX(AT14:AT17)-MIN(AT14:AT17)+1</f>
         <v>1</v>
       </c>
-      <c r="AY18" s="118">
+      <c r="AY18" s="129">
         <v>53</v>
       </c>
       <c r="AZ18" s="28" t="str">
@@ -31855,7 +31887,7 @@
       <c r="BS18" s="25"/>
       <c r="BT18" s="25"/>
     </row>
-    <row r="19" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72" ht="15" customHeight="1">
       <c r="A19" s="18">
         <v>13</v>
       </c>
@@ -31928,7 +31960,7 @@
         <f>MIN(AI14:AI17)</f>
         <v>0</v>
       </c>
-      <c r="AY19" s="119"/>
+      <c r="AY19" s="130"/>
       <c r="AZ19" s="31" t="str">
         <f>AO39</f>
         <v>2F</v>
@@ -31957,7 +31989,7 @@
       <c r="BS19" s="25"/>
       <c r="BT19" s="25"/>
     </row>
-    <row r="20" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72" ht="15" customHeight="1">
       <c r="A20" s="18">
         <v>14</v>
       </c>
@@ -32129,7 +32161,7 @@
       <c r="BB20" s="25"/>
       <c r="BC20" s="36"/>
       <c r="BD20" s="25"/>
-      <c r="BE20" s="118">
+      <c r="BE20" s="129">
         <v>58</v>
       </c>
       <c r="BF20" s="28" t="str">
@@ -32151,7 +32183,7 @@
       <c r="BS20" s="25"/>
       <c r="BT20" s="25"/>
     </row>
-    <row r="21" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72" ht="15" customHeight="1">
       <c r="A21" s="18">
         <v>15</v>
       </c>
@@ -32326,7 +32358,7 @@
       <c r="BB21" s="35"/>
       <c r="BC21" s="36"/>
       <c r="BD21" s="39"/>
-      <c r="BE21" s="119"/>
+      <c r="BE21" s="130"/>
       <c r="BF21" s="31" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -32346,7 +32378,7 @@
       <c r="BS21" s="25"/>
       <c r="BT21" s="25"/>
     </row>
-    <row r="22" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72" ht="15" customHeight="1">
       <c r="A22" s="18">
         <v>16</v>
       </c>
@@ -32508,7 +32540,7 @@
         <f>AR22-AS22</f>
         <v>0</v>
       </c>
-      <c r="AY22" s="118">
+      <c r="AY22" s="129">
         <v>54</v>
       </c>
       <c r="AZ22" s="28" t="str">
@@ -32539,7 +32571,7 @@
       <c r="BS22" s="25"/>
       <c r="BT22" s="35"/>
     </row>
-    <row r="23" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72" ht="15" customHeight="1">
       <c r="A23" s="18">
         <v>17</v>
       </c>
@@ -32701,7 +32733,7 @@
         <f>AR23-AS23</f>
         <v>0</v>
       </c>
-      <c r="AY23" s="119"/>
+      <c r="AY23" s="130"/>
       <c r="AZ23" s="31" t="str">
         <f>AO51</f>
         <v>2H</v>
@@ -32722,7 +32754,7 @@
       <c r="BN23" s="25"/>
       <c r="BO23" s="36"/>
       <c r="BP23" s="25"/>
-      <c r="BQ23" s="118">
+      <c r="BQ23" s="129">
         <v>64</v>
       </c>
       <c r="BR23" s="28" t="str">
@@ -32732,7 +32764,7 @@
       <c r="BS23" s="29"/>
       <c r="BT23" s="30"/>
     </row>
-    <row r="24" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72" ht="15" customHeight="1">
       <c r="A24" s="18">
         <v>18</v>
       </c>
@@ -32891,7 +32923,7 @@
       <c r="BN24" s="25"/>
       <c r="BO24" s="36"/>
       <c r="BP24" s="39"/>
-      <c r="BQ24" s="119"/>
+      <c r="BQ24" s="130"/>
       <c r="BR24" s="31" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -32899,7 +32931,7 @@
       <c r="BS24" s="32"/>
       <c r="BT24" s="33"/>
     </row>
-    <row r="25" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:72" ht="15" customHeight="1">
       <c r="A25" s="18">
         <v>19</v>
       </c>
@@ -32998,7 +33030,7 @@
       <c r="BS25" s="25"/>
       <c r="BT25" s="25"/>
     </row>
-    <row r="26" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72" ht="15" customHeight="1">
       <c r="A26" s="18">
         <v>20</v>
       </c>
@@ -33164,7 +33196,7 @@
         <f>AR26-AS26</f>
         <v>0</v>
       </c>
-      <c r="AY26" s="118">
+      <c r="AY26" s="129">
         <v>51</v>
       </c>
       <c r="AZ26" s="28" t="str">
@@ -33192,7 +33224,7 @@
       <c r="BS26" s="25"/>
       <c r="BT26" s="25"/>
     </row>
-    <row r="27" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:72" ht="15" customHeight="1">
       <c r="A27" s="18">
         <v>21</v>
       </c>
@@ -33358,7 +33390,7 @@
         <f>AR27-AS27</f>
         <v>0</v>
       </c>
-      <c r="AY27" s="119"/>
+      <c r="AY27" s="130"/>
       <c r="AZ27" s="31" t="str">
         <f>AO9</f>
         <v>2A</v>
@@ -33387,7 +33419,7 @@
       <c r="BS27" s="25"/>
       <c r="BT27" s="25"/>
     </row>
-    <row r="28" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:72" ht="15" customHeight="1">
       <c r="A28" s="18">
         <v>22</v>
       </c>
@@ -33555,7 +33587,7 @@
       <c r="BB28" s="25"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="25"/>
-      <c r="BE28" s="118">
+      <c r="BE28" s="129">
         <v>59</v>
       </c>
       <c r="BF28" s="28" t="str">
@@ -33577,7 +33609,7 @@
       <c r="BS28" s="25"/>
       <c r="BT28" s="25"/>
     </row>
-    <row r="29" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:72" ht="15" customHeight="1">
       <c r="A29" s="18">
         <v>23</v>
       </c>
@@ -33748,7 +33780,7 @@
       <c r="BB29" s="35"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="39"/>
-      <c r="BE29" s="119"/>
+      <c r="BE29" s="130"/>
       <c r="BF29" s="31" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -33768,7 +33800,7 @@
       <c r="BS29" s="25"/>
       <c r="BT29" s="25"/>
     </row>
-    <row r="30" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72" ht="15" customHeight="1">
       <c r="A30" s="18">
         <v>24</v>
       </c>
@@ -33910,7 +33942,7 @@
         <f>MAX(AT26:AT29)-MIN(AT26:AT29)+1</f>
         <v>1</v>
       </c>
-      <c r="AY30" s="118">
+      <c r="AY30" s="129">
         <v>52</v>
       </c>
       <c r="AZ30" s="28" t="str">
@@ -33938,7 +33970,7 @@
       <c r="BS30" s="25"/>
       <c r="BT30" s="25"/>
     </row>
-    <row r="31" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:72" ht="15" customHeight="1">
       <c r="A31" s="18">
         <v>25</v>
       </c>
@@ -34004,7 +34036,7 @@
         <f>MIN(AI26:AI29)</f>
         <v>0</v>
       </c>
-      <c r="AY31" s="119"/>
+      <c r="AY31" s="130"/>
       <c r="AZ31" s="31" t="str">
         <f>AO21</f>
         <v>2C</v>
@@ -34028,15 +34060,15 @@
       <c r="BN31" s="35"/>
       <c r="BO31" s="36"/>
       <c r="BP31" s="41"/>
-      <c r="BQ31" s="124" t="str">
+      <c r="BQ31" s="131" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BR31" s="125"/>
-      <c r="BS31" s="125"/>
-      <c r="BT31" s="126"/>
+      <c r="BR31" s="132"/>
+      <c r="BS31" s="132"/>
+      <c r="BT31" s="133"/>
     </row>
-    <row r="32" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72" ht="15" customHeight="1">
       <c r="A32" s="18">
         <v>26</v>
       </c>
@@ -34214,7 +34246,7 @@
       <c r="BH32" s="25"/>
       <c r="BI32" s="36"/>
       <c r="BJ32" s="25"/>
-      <c r="BK32" s="118">
+      <c r="BK32" s="129">
         <v>62</v>
       </c>
       <c r="BL32" s="28" t="str">
@@ -34225,12 +34257,12 @@
       <c r="BN32" s="30"/>
       <c r="BO32" s="40"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="127"/>
-      <c r="BR32" s="128"/>
-      <c r="BS32" s="128"/>
-      <c r="BT32" s="129"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="135"/>
+      <c r="BS32" s="135"/>
+      <c r="BT32" s="136"/>
     </row>
-    <row r="33" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:72" ht="15" customHeight="1">
       <c r="A33" s="18">
         <v>27</v>
       </c>
@@ -34411,7 +34443,7 @@
       <c r="BH33" s="25"/>
       <c r="BI33" s="36"/>
       <c r="BJ33" s="39"/>
-      <c r="BK33" s="119"/>
+      <c r="BK33" s="130"/>
       <c r="BL33" s="31" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -34425,7 +34457,7 @@
       <c r="BS33" s="25"/>
       <c r="BT33" s="25"/>
     </row>
-    <row r="34" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:72" ht="15" customHeight="1">
       <c r="A34" s="18">
         <v>28</v>
       </c>
@@ -34587,7 +34619,7 @@
         <f>AR34-AS34</f>
         <v>0</v>
       </c>
-      <c r="AY34" s="118">
+      <c r="AY34" s="129">
         <v>55</v>
       </c>
       <c r="AZ34" s="28" t="str">
@@ -34618,7 +34650,7 @@
       <c r="BS34" s="25"/>
       <c r="BT34" s="35"/>
     </row>
-    <row r="35" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:72" ht="15" customHeight="1">
       <c r="A35" s="18">
         <v>29</v>
       </c>
@@ -34780,7 +34812,7 @@
         <f>AR35-AS35</f>
         <v>0</v>
       </c>
-      <c r="AY35" s="119"/>
+      <c r="AY35" s="130"/>
       <c r="AZ35" s="31" t="str">
         <f>AO33</f>
         <v>2E</v>
@@ -34804,7 +34836,7 @@
       <c r="BN35" s="25"/>
       <c r="BO35" s="25"/>
       <c r="BP35" s="25"/>
-      <c r="BQ35" s="118">
+      <c r="BQ35" s="129">
         <v>63</v>
       </c>
       <c r="BR35" s="28" t="str">
@@ -34814,7 +34846,7 @@
       <c r="BS35" s="29"/>
       <c r="BT35" s="30"/>
     </row>
-    <row r="36" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:72" ht="15" customHeight="1">
       <c r="A36" s="18">
         <v>30</v>
       </c>
@@ -34962,7 +34994,7 @@
       <c r="BB36" s="25"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="25"/>
-      <c r="BE36" s="118">
+      <c r="BE36" s="129">
         <v>60</v>
       </c>
       <c r="BF36" s="28" t="str">
@@ -34979,7 +35011,7 @@
       <c r="BN36" s="25"/>
       <c r="BO36" s="25"/>
       <c r="BP36" s="25"/>
-      <c r="BQ36" s="119"/>
+      <c r="BQ36" s="130"/>
       <c r="BR36" s="31" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -34987,7 +35019,7 @@
       <c r="BS36" s="32"/>
       <c r="BT36" s="33"/>
     </row>
-    <row r="37" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72" ht="15" customHeight="1">
       <c r="A37" s="18">
         <v>31</v>
       </c>
@@ -35062,7 +35094,7 @@
       <c r="BB37" s="35"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="39"/>
-      <c r="BE37" s="119"/>
+      <c r="BE37" s="130"/>
       <c r="BF37" s="31" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -35082,7 +35114,7 @@
       <c r="BS37" s="25"/>
       <c r="BT37" s="25"/>
     </row>
-    <row r="38" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:72" ht="15" customHeight="1">
       <c r="A38" s="18">
         <v>32</v>
       </c>
@@ -35248,7 +35280,7 @@
         <f>AR38-AS38</f>
         <v>0</v>
       </c>
-      <c r="AY38" s="118">
+      <c r="AY38" s="129">
         <v>56</v>
       </c>
       <c r="AZ38" s="28" t="str">
@@ -35272,7 +35304,7 @@
       <c r="BS38" s="25"/>
       <c r="BT38" s="25"/>
     </row>
-    <row r="39" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:72" ht="15" customHeight="1">
       <c r="A39" s="18">
         <v>33</v>
       </c>
@@ -35438,7 +35470,7 @@
         <f>AR39-AS39</f>
         <v>0</v>
       </c>
-      <c r="AY39" s="119"/>
+      <c r="AY39" s="130"/>
       <c r="AZ39" s="31" t="str">
         <f>AO45</f>
         <v>2G</v>
@@ -35458,7 +35490,7 @@
       <c r="BS39" s="25"/>
       <c r="BT39" s="25"/>
     </row>
-    <row r="40" spans="1:72" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:72" ht="15" customHeight="1" thickBot="1">
       <c r="A40" s="18">
         <v>34</v>
       </c>
@@ -35621,7 +35653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:72" ht="15" customHeight="1">
       <c r="A41" s="18">
         <v>35</v>
       </c>
@@ -35783,25 +35815,25 @@
         <f>AR41-AS41</f>
         <v>0</v>
       </c>
-      <c r="BJ41" s="120" t="str">
+      <c r="BJ41" s="146" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BK41" s="120"/>
-      <c r="BL41" s="120"/>
-      <c r="BM41" s="120"/>
-      <c r="BN41" s="120"/>
-      <c r="BO41" s="122" t="str">
+      <c r="BK41" s="146"/>
+      <c r="BL41" s="146"/>
+      <c r="BM41" s="146"/>
+      <c r="BN41" s="146"/>
+      <c r="BO41" s="148" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BP41" s="122"/>
-      <c r="BQ41" s="122"/>
-      <c r="BR41" s="122"/>
-      <c r="BS41" s="122"/>
-      <c r="BT41" s="122"/>
+      <c r="BP41" s="148"/>
+      <c r="BQ41" s="148"/>
+      <c r="BR41" s="148"/>
+      <c r="BS41" s="148"/>
+      <c r="BT41" s="148"/>
     </row>
-    <row r="42" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:72" ht="15" customHeight="1">
       <c r="A42" s="18">
         <v>36</v>
       </c>
@@ -35943,19 +35975,19 @@
         <f>MAX(AT38:AT41)-MIN(AT38:AT41)+1</f>
         <v>1</v>
       </c>
-      <c r="BJ42" s="121"/>
-      <c r="BK42" s="121"/>
-      <c r="BL42" s="121"/>
-      <c r="BM42" s="121"/>
-      <c r="BN42" s="121"/>
-      <c r="BO42" s="123"/>
-      <c r="BP42" s="123"/>
-      <c r="BQ42" s="123"/>
-      <c r="BR42" s="123"/>
-      <c r="BS42" s="123"/>
-      <c r="BT42" s="123"/>
+      <c r="BJ42" s="147"/>
+      <c r="BK42" s="147"/>
+      <c r="BL42" s="147"/>
+      <c r="BM42" s="147"/>
+      <c r="BN42" s="147"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="149"/>
+      <c r="BS42" s="149"/>
+      <c r="BT42" s="149"/>
     </row>
-    <row r="43" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:72" ht="15" customHeight="1">
       <c r="A43" s="18">
         <v>37</v>
       </c>
@@ -36023,7 +36055,7 @@
       </c>
       <c r="AY43" s="80"/>
     </row>
-    <row r="44" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:72" ht="15" customHeight="1">
       <c r="A44" s="18">
         <v>38</v>
       </c>
@@ -36190,7 +36222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72" ht="15" customHeight="1">
       <c r="A45" s="18">
         <v>39</v>
       </c>
@@ -36357,7 +36389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:72" ht="15" customHeight="1">
       <c r="A46" s="18">
         <v>40</v>
       </c>
@@ -36519,14 +36551,14 @@
         <f>AR46-AS46</f>
         <v>0</v>
       </c>
-      <c r="AY46" s="109" t="s">
+      <c r="AY46" s="137" t="s">
         <v>2231</v>
       </c>
-      <c r="AZ46" s="110"/>
-      <c r="BA46" s="110"/>
-      <c r="BB46" s="111"/>
+      <c r="AZ46" s="138"/>
+      <c r="BA46" s="138"/>
+      <c r="BB46" s="139"/>
     </row>
-    <row r="47" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:72" ht="15" customHeight="1">
       <c r="A47" s="18">
         <v>41</v>
       </c>
@@ -36688,12 +36720,12 @@
         <f>AR47-AS47</f>
         <v>0</v>
       </c>
-      <c r="AY47" s="112"/>
-      <c r="AZ47" s="113"/>
-      <c r="BA47" s="113"/>
-      <c r="BB47" s="114"/>
+      <c r="AY47" s="140"/>
+      <c r="AZ47" s="141"/>
+      <c r="BA47" s="141"/>
+      <c r="BB47" s="142"/>
     </row>
-    <row r="48" spans="1:72" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:72" ht="15" customHeight="1">
       <c r="A48" s="18">
         <v>42</v>
       </c>
@@ -36835,12 +36867,12 @@
         <f>MAX(AT44:AT47)-MIN(AT44:AT47)+1</f>
         <v>1</v>
       </c>
-      <c r="AY48" s="112"/>
-      <c r="AZ48" s="113"/>
-      <c r="BA48" s="113"/>
-      <c r="BB48" s="114"/>
+      <c r="AY48" s="140"/>
+      <c r="AZ48" s="141"/>
+      <c r="BA48" s="141"/>
+      <c r="BB48" s="142"/>
     </row>
-    <row r="49" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:54" ht="15" customHeight="1">
       <c r="A49" s="18">
         <v>43</v>
       </c>
@@ -36906,12 +36938,12 @@
         <f>MIN(AI44:AI47)</f>
         <v>0</v>
       </c>
-      <c r="AY49" s="112"/>
-      <c r="AZ49" s="113"/>
-      <c r="BA49" s="113"/>
-      <c r="BB49" s="114"/>
+      <c r="AY49" s="140"/>
+      <c r="AZ49" s="141"/>
+      <c r="BA49" s="141"/>
+      <c r="BB49" s="142"/>
     </row>
-    <row r="50" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:54" ht="15" customHeight="1">
       <c r="A50" s="18">
         <v>44</v>
       </c>
@@ -37077,12 +37109,12 @@
         <f>AR50-AS50</f>
         <v>0</v>
       </c>
-      <c r="AY50" s="112"/>
-      <c r="AZ50" s="113"/>
-      <c r="BA50" s="113"/>
-      <c r="BB50" s="114"/>
+      <c r="AY50" s="140"/>
+      <c r="AZ50" s="141"/>
+      <c r="BA50" s="141"/>
+      <c r="BB50" s="142"/>
     </row>
-    <row r="51" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:54" ht="15" customHeight="1">
       <c r="A51" s="18">
         <v>45</v>
       </c>
@@ -37248,12 +37280,12 @@
         <f>AR51-AS51</f>
         <v>0</v>
       </c>
-      <c r="AY51" s="112"/>
-      <c r="AZ51" s="113"/>
-      <c r="BA51" s="113"/>
-      <c r="BB51" s="114"/>
+      <c r="AY51" s="140"/>
+      <c r="AZ51" s="141"/>
+      <c r="BA51" s="141"/>
+      <c r="BB51" s="142"/>
     </row>
-    <row r="52" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:54" ht="15" customHeight="1">
       <c r="A52" s="18">
         <v>46</v>
       </c>
@@ -37415,12 +37447,12 @@
         <f>AR52-AS52</f>
         <v>0</v>
       </c>
-      <c r="AY52" s="115"/>
-      <c r="AZ52" s="116"/>
-      <c r="BA52" s="116"/>
-      <c r="BB52" s="117"/>
+      <c r="AY52" s="143"/>
+      <c r="AZ52" s="144"/>
+      <c r="BA52" s="144"/>
+      <c r="BB52" s="145"/>
     </row>
-    <row r="53" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:54" ht="15" customHeight="1">
       <c r="A53" s="18">
         <v>47</v>
       </c>
@@ -37583,7 +37615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:54" ht="15" customHeight="1">
       <c r="A54" s="44">
         <v>48</v>
       </c>
@@ -37726,7 +37758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:54">
       <c r="A55" s="49"/>
       <c r="B55" s="50"/>
       <c r="C55" s="49"/>
@@ -37752,9 +37784,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:54" ht="12.75" customHeight="1"/>
+    <row r="57" spans="1:54" ht="12.75" customHeight="1"/>
+    <row r="58" spans="1:54">
       <c r="R58" s="58">
         <f>DATE(2018,6,30)+TIME(7,0,0)+gmt_delta</f>
         <v>43281.75</v>
@@ -37768,7 +37800,7 @@
         <v>W49</v>
       </c>
     </row>
-    <row r="59" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:54" ht="12.75" customHeight="1">
       <c r="R59" s="58">
         <f>DATE(2018,6,30)+TIME(3,0,0)+gmt_delta</f>
         <v>43281.583333333336</v>
@@ -37782,7 +37814,7 @@
         <v>W50</v>
       </c>
     </row>
-    <row r="60" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:54" ht="12.75" customHeight="1">
       <c r="R60" s="58">
         <f>DATE(2018,7,1)+TIME(3,0,0)+gmt_delta</f>
         <v>43282.583333333336</v>
@@ -37796,7 +37828,7 @@
         <v>W51</v>
       </c>
     </row>
-    <row r="61" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:54" ht="12.75" customHeight="1">
       <c r="R61" s="58">
         <f>DATE(2018,7,1)+TIME(7,0,0)+gmt_delta</f>
         <v>43282.75</v>
@@ -37810,7 +37842,7 @@
         <v>W52</v>
       </c>
     </row>
-    <row r="62" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:54" ht="12.75" customHeight="1">
       <c r="R62" s="58">
         <f>DATE(2018,7,2)+TIME(3,0,0)+gmt_delta</f>
         <v>43283.583333333336</v>
@@ -37824,7 +37856,7 @@
         <v>W53</v>
       </c>
     </row>
-    <row r="63" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:54" ht="12.75" customHeight="1">
       <c r="R63" s="58">
         <f>DATE(2018,7,2)+TIME(7,0,0)+gmt_delta</f>
         <v>43283.75</v>
@@ -37838,7 +37870,7 @@
         <v>W54</v>
       </c>
     </row>
-    <row r="64" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:54" ht="12.75" customHeight="1">
       <c r="R64" s="58">
         <f>DATE(2018,7,3)+TIME(3,0,0)+gmt_delta</f>
         <v>43284.583333333336</v>
@@ -37852,7 +37884,7 @@
         <v>W55</v>
       </c>
     </row>
-    <row r="65" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="18:26" ht="12.75" customHeight="1">
       <c r="R65" s="58">
         <f>DATE(2018,7,3)+TIME(7,0,0)+gmt_delta</f>
         <v>43284.75</v>
@@ -37866,10 +37898,10 @@
         <v>W56</v>
       </c>
     </row>
-    <row r="66" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="67" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="68" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="69" spans="18:26" ht="12.75" customHeight="1">
       <c r="R69" s="58">
         <f>DATE(2018,7,6)+TIME(3,0,0)+gmt_delta</f>
         <v>43287.583333333336</v>
@@ -37883,7 +37915,7 @@
         <v>W57</v>
       </c>
     </row>
-    <row r="70" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="18:26" ht="12.75" customHeight="1">
       <c r="R70" s="58">
         <f>DATE(2018,7,6)+TIME(7,0,0)+gmt_delta</f>
         <v>43287.75</v>
@@ -37897,7 +37929,7 @@
         <v>W58</v>
       </c>
     </row>
-    <row r="71" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="18:26" ht="12.75" customHeight="1">
       <c r="R71" s="58">
         <f>DATE(2018,7,7)+TIME(3,0,0)+gmt_delta</f>
         <v>43288.583333333336</v>
@@ -37911,7 +37943,7 @@
         <v>W59</v>
       </c>
     </row>
-    <row r="72" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="18:26" ht="12.75" customHeight="1">
       <c r="R72" s="58">
         <f>DATE(2018,7,7)+TIME(7,0,0)+gmt_delta</f>
         <v>43288.75</v>
@@ -37925,10 +37957,10 @@
         <v>W60</v>
       </c>
     </row>
-    <row r="73" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="74" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="75" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="76" spans="18:26" ht="12.75" customHeight="1">
       <c r="R76" s="58">
         <f>DATE(2018,7,10)+TIME(7,0,0)+gmt_delta</f>
         <v>43291.75</v>
@@ -37950,7 +37982,7 @@
         <v>L61</v>
       </c>
     </row>
-    <row r="77" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="18:26" ht="12.75" customHeight="1">
       <c r="R77" s="58">
         <f>DATE(2018,7,11)+TIME(7,0,0)+gmt_delta</f>
         <v>43292.75</v>
@@ -37972,9 +38004,9 @@
         <v>L62</v>
       </c>
     </row>
-    <row r="79" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="18:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="80" spans="18:26" ht="12.75" customHeight="1"/>
+    <row r="81" spans="18:20">
       <c r="R81" s="58">
         <f>DATE(2018,7,14)+TIME(3,0,0)+gmt_delta</f>
         <v>43295.583333333336</v>
@@ -37984,9 +38016,9 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="18:20" ht="12.75" customHeight="1"/>
+    <row r="84" spans="18:20" ht="12.75" customHeight="1"/>
+    <row r="85" spans="18:20">
       <c r="R85" s="58">
         <f>DATE(2018,7,15)+TIME(4,0,0)+gmt_delta</f>
         <v>43296.625</v>
@@ -38000,34 +38032,13 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="18:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="18:20" ht="12.75" customHeight="1"/>
+    <row r="88" spans="18:20" ht="12.75" customHeight="1"/>
+    <row r="96" spans="18:20" ht="12.75" customHeight="1"/>
+    <row r="97" ht="12.75" customHeight="1"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="PAglMCMPk026QNImqs5vht8iXkHMK+l+My+2rfGLtRZkio8JaaxdUcv1sFv6JUjNu8x8GCTRGfRxZo4OzEC8MA==" saltValue="oAWGgK7w1lThPFYybvkV5g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BQ6:BT7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="AY10:AY11"/>
-    <mergeCell ref="BE12:BE13"/>
-    <mergeCell ref="AY6:BB7"/>
-    <mergeCell ref="BE6:BH7"/>
-    <mergeCell ref="BK6:BN7"/>
-    <mergeCell ref="AY22:AY23"/>
-    <mergeCell ref="BQ23:BQ24"/>
-    <mergeCell ref="AY18:AY19"/>
-    <mergeCell ref="BE20:BE21"/>
-    <mergeCell ref="AY14:AY15"/>
-    <mergeCell ref="BK16:BK17"/>
-    <mergeCell ref="AY30:AY31"/>
-    <mergeCell ref="BQ31:BT32"/>
-    <mergeCell ref="BK32:BK33"/>
-    <mergeCell ref="AY26:AY27"/>
-    <mergeCell ref="BE28:BE29"/>
     <mergeCell ref="AY46:BB52"/>
     <mergeCell ref="AY38:AY39"/>
     <mergeCell ref="BJ41:BN42"/>
@@ -38035,6 +38046,27 @@
     <mergeCell ref="BQ35:BQ36"/>
     <mergeCell ref="BE36:BE37"/>
     <mergeCell ref="BO41:BT42"/>
+    <mergeCell ref="AY30:AY31"/>
+    <mergeCell ref="BQ31:BT32"/>
+    <mergeCell ref="BK32:BK33"/>
+    <mergeCell ref="AY26:AY27"/>
+    <mergeCell ref="BE28:BE29"/>
+    <mergeCell ref="AY22:AY23"/>
+    <mergeCell ref="BQ23:BQ24"/>
+    <mergeCell ref="AY18:AY19"/>
+    <mergeCell ref="BE20:BE21"/>
+    <mergeCell ref="AY14:AY15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="AY10:AY11"/>
+    <mergeCell ref="BE12:BE13"/>
+    <mergeCell ref="AY6:BB7"/>
+    <mergeCell ref="BE6:BH7"/>
+    <mergeCell ref="BK6:BN7"/>
+    <mergeCell ref="BQ6:BT7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F55">
     <cfRule type="expression" dxfId="99" priority="16" stopIfTrue="1">
@@ -38451,25 +38483,198 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB10:BB11 BB14:BB15 BB26:BB27 BB30:BB31 BB18:BB19 BB22:BB23 BB34:BB35 BB38:BB39 BH12:BH13 BH20:BH21 BH28:BH29 BH36:BH37 BN16:BN17 BN32:BN33 BT23:BT24 BT35:BT36" xr:uid="{5DC19248-CA97-4A65-901D-902A8CFD1871}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB10:BB11 BB14:BB15 BB26:BB27 BB30:BB31 BB18:BB19 BB22:BB23 BB34:BB35 BB38:BB39 BH12:BH13 BH20:BH21 BH28:BH29 BH36:BH37 BN16:BN17 BN32:BN33 BT23:BT24 BT35:BT36">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G55 BA26:BA27 BA10:BA11 BA14:BA15 BA30:BA31 BA18:BA19 BA22:BA23 BA34:BA35 BA38:BA39 BG12:BG13 BG20:BG21 BG28:BG29 BG36:BG37 BM16:BM17 BM32:BM33 BS23:BS24 BS35:BS36" xr:uid="{C7F7E835-588F-4CFE-8B58-3E549F511EDD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G55 BA26:BA27 BA10:BA11 BA14:BA15 BA30:BA31 BA18:BA19 BA22:BA23 BA34:BA35 BA38:BA39 BG12:BG13 BG20:BG21 BG28:BG29 BG36:BG37 BM16:BM17 BM32:BM33 BS23:BS24 BS35:BS36">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="O3" location="Settings!C4" tooltip="Settings" display="Settings!C4" xr:uid="{B7D43826-7A10-4B1F-B7E9-9C5EA92B5AE3}"/>
-    <hyperlink ref="J5:P5" r:id="rId1" tooltip="Excel Schedule" display="Home Page: www.excely.com" xr:uid="{F1B16304-7A83-4C19-8499-62AB6ADF14F7}"/>
-    <hyperlink ref="J5:P6" r:id="rId2" tooltip="World Cup 2018 Schedule in Excel" display="Home Page: www.excely.com" xr:uid="{C5C0CB06-50F0-4DD5-AAB0-434A0F623240}"/>
-    <hyperlink ref="AY46:BB52" r:id="rId3" tooltip="FIFA World Cup Historical Data 1930 - 2014" display="http://www.excely.com/football/fifa-world-cup-statistics.shtml" xr:uid="{3D7E925C-71F7-4395-AF7F-647ABF98F356}"/>
+    <hyperlink ref="O3" location="Settings!C4" tooltip="Settings" display="Settings!C4"/>
+    <hyperlink ref="J5:P5" r:id="rId1" tooltip="Excel Schedule" display="Home Page: www.excely.com"/>
+    <hyperlink ref="J5:P6" r:id="rId2" tooltip="World Cup 2018 Schedule in Excel" display="Home Page: www.excely.com"/>
+    <hyperlink ref="AY46:BB52" r:id="rId3" tooltip="FIFA World Cup Historical Data 1930 - 2014" display="http://www.excely.com/football/fifa-world-cup-statistics.shtml"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="48" orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;Cwww.excely.com (c) 2018</oddFooter>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId4"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="150" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F1" s="150" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="150" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F2" s="150" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="150" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F3" s="150" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="150" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F4" s="150" t="s">
+        <v>2175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="150" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F5" s="150" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="150" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F6" s="150" t="s">
+        <v>2173</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
+      <c r="A7" s="150" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F7" s="150" t="s">
+        <v>2179</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="150" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F8" s="150" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="150" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2560</v>
+      </c>
+      <c r="F9" s="150" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="150" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30">
+      <c r="A11" s="150" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="150" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>